<commit_message>
Reviewing Project management matters: - Update meeting minutes - Add deliverable checklist
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -119,7 +119,7 @@
     <t>In progress: 33-65 (%)</t>
   </si>
   <si>
-    <t>Started: 0-33 (%)</t>
+    <t>Starting: 0-33 (%)</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -330,6 +330,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -393,21 +396,340 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="107">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -504,6 +826,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -594,22 +946,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,91 +1028,45 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -856,6 +1149,37 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -926,6 +1250,50 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -971,26 +1339,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1384,407 +1732,436 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="13"/>
-    <col min="5" max="5" width="21.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="12"/>
+    <col min="1" max="1" width="7.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="13"/>
     <col min="8" max="16384" width="22.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="19">
         <v>40635</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="20">
         <v>40635</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="20">
         <v>40635</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="21">
         <v>40642</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="19">
         <v>40768</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="20">
         <v>40768</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="20">
         <v>40768</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="20">
         <v>40768</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="21">
         <v>40768</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="10"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="20">
         <v>40915</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="20">
         <v>40915</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="20">
         <v>40915</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
         <f t="shared" ref="A14:A17" si="1">A13+1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="20">
         <v>40915</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="20">
         <v>40915</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="20">
         <v>40915</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="21">
         <v>40915</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="10"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Started">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Started">
       <formula>NOT(ISERROR(SEARCH("Started",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="In progress">
+      <formula>NOT(ISERROR(SEARCH("In progress",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="6" operator="containsText" text="Finalizing">
+      <formula>NOT(ISERROR(SEARCH("Finalizing",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="Start">
+      <formula>NOT(ISERROR(SEARCH("Start",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="17" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="16" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="15" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
       <formula>$B$2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="50" priority="13" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Phase 2">
+    <cfRule type="containsText" dxfId="48" priority="11" operator="containsText" text="Phase 2">
       <formula>NOT(ISERROR(SEARCH("Phase 2",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Phase 3">
+    <cfRule type="containsText" dxfId="47" priority="10" operator="containsText" text="Phase 3">
       <formula>NOT(ISERROR(SEARCH("Phase 3",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="46" priority="9" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+      <formula>"Not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"Not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"Not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="600" yWindow="234" count="1">
@@ -1855,7 +2232,7 @@
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to-do for each deliverable
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>Phase</t>
   </si>
@@ -122,6 +122,12 @@
     <t>Detailed Design Specs 
 (one per use case):
 - Sequence Diagram + Object Detailed Specs</t>
+  </si>
+  <si>
+    <t>Need to do review :
++ review form (if there's changes)
++ audit meeting minutes
++ Update recordlogs.xls with the new file location</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,228 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -790,11 +1017,11 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="7" bestFit="1" customWidth="1"/>
@@ -802,11 +1029,11 @@
     <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" style="7" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="7"/>
+    <col min="7" max="7" width="36.140625" style="7" customWidth="1"/>
     <col min="8" max="16384" width="22.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -829,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -846,9 +1073,11 @@
         <v>28</v>
       </c>
       <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <f>A2+1</f>
         <v>2</v>
@@ -866,9 +1095,11 @@
         <v>28</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <f>A3+1</f>
         <v>3</v>
@@ -890,7 +1121,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>4</v>
@@ -912,7 +1143,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -930,9 +1161,11 @@
         <v>28</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -950,9 +1183,11 @@
         <v>28</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -970,9 +1205,11 @@
         <v>28</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -990,9 +1227,11 @@
         <v>28</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1034,7 +1273,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1054,7 +1293,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1074,7 +1313,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <f t="shared" ref="A14:A17" si="1">A13+1</f>
         <v>13</v>
@@ -1094,7 +1333,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1114,7 +1353,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1134,7 +1373,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1157,75 +1396,80 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Started">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Started">
       <formula>NOT(ISERROR(SEARCH("Started",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Finalizing">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="Finalizing">
       <formula>NOT(ISERROR(SEARCH("Finalizing",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Start">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Start">
       <formula>NOT(ISERROR(SEARCH("Start",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="18" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="15" operator="equal">
       <formula>$B$2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Phase 2">
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="Phase 2">
       <formula>NOT(ISERROR(SEARCH("Phase 2",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Phase 3">
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Phase 3">
       <formula>NOT(ISERROR(SEARCH("Phase 3",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"Not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="600" yWindow="234" count="1">

</xml_diff>

<commit_message>
update Prototyping Study Report to be ready for printing
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -256,27 +256,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -470,74 +450,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -551,7 +463,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="363636"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -837,7 +749,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11:E17"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1028,7 +940,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1046,8 +958,8 @@
         <v>28</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="15" t="s">
-        <v>33</v>
+      <c r="G9" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1215,79 +1127,79 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="Started">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Started">
       <formula>NOT(ISERROR(SEARCH("Started",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="Finalizing">
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="Finalizing">
       <formula>NOT(ISERROR(SEARCH("Finalizing",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="Start">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Start">
       <formula>NOT(ISERROR(SEARCH("Start",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>$B$2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Phase 2">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Phase 2">
       <formula>NOT(ISERROR(SEARCH("Phase 2",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Phase 3">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Phase 3">
       <formula>NOT(ISERROR(SEARCH("Phase 3",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",G1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update status for High Level Design Spec
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -749,7 +749,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -936,8 +936,8 @@
         <v>28</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="15" t="s">
-        <v>33</v>
+      <c r="G8" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update test + dev plan Add user guide folder Update SIT test case
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -855,9 +855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">

</xml_diff>

<commit_message>
Project deliverables completed !
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
+++ b/docs/PM-1 Project Management/PM-1.5 Project Deliverables/vms_pm15_Deliverables_CheckList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
   <si>
     <t>Phase</t>
   </si>
@@ -249,7 +249,307 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -484,6 +784,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -497,7 +865,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="363636"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -781,9 +1149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -821,7 +1189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1033,10 +1401,12 @@
         <v>40915</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
@@ -1095,10 +1465,12 @@
         <v>40915</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
@@ -1114,11 +1486,13 @@
       <c r="D15" s="16">
         <v>40915</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
+      <c r="E15" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
@@ -1134,11 +1508,13 @@
       <c r="D16" s="16">
         <v>40915</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>27</v>
+      <c r="E16" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
@@ -1155,87 +1531,89 @@
         <v>40915</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="Start">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Start">
       <formula>NOT(ISERROR(SEARCH("Start",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Finalizing">
+    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="Finalizing">
       <formula>NOT(ISERROR(SEARCH("Finalizing",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Started">
+    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Started">
       <formula>NOT(ISERROR(SEARCH("Started",E1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="19" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="18" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="16" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Phase 3">
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="Phase 3">
       <formula>NOT(ISERROR(SEARCH("Phase 3",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="Phase 2">
+    <cfRule type="containsText" dxfId="44" priority="12" operator="containsText" text="Phase 2">
       <formula>NOT(ISERROR(SEARCH("Phase 2",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="43" priority="13" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="42" priority="14" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="equal">
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"Not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1275,7 +1653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
@@ -1350,22 +1728,22 @@
   </sheetData>
   <autoFilter ref="A1:C3"/>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Phase 3">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Phase 3">
       <formula>NOT(ISERROR(SEARCH("Phase 3",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Phase 2">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Phase 2">
       <formula>NOT(ISERROR(SEARCH("Phase 2",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Phase 1">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Phase 1">
       <formula>NOT(ISERROR(SEARCH("Phase 1",A1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>